<commit_message>
Update the sprint 2 requirements stack
</commit_message>
<xml_diff>
--- a/Documentation/Sprint 2/Requirements/Requirements Stack.xlsx
+++ b/Documentation/Sprint 2/Requirements/Requirements Stack.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StardewModding\EECS-581-Group-7-Project-3\Documentation\Sprint 2\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041223AA-8C34-47B4-8F83-A3C212E0E24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE3BF4D-6E0D-49EC-836A-2DECBC129148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -62,9 +62,6 @@
     <t>There shouldn't be a shift the layout when many class cards have been added (should be able to scroll)</t>
   </si>
   <si>
-    <t>Total should be updated dynamically as classes are added/removed</t>
-  </si>
-  <si>
     <t>2.3</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>Some large requirements were split into smaller component requirements which were then assigned their own story points. A 'S' indicates that the requirement has been split in this way and its complexity is represented by the story points of its components.</t>
   </si>
   <si>
-    <t>The system should display the total number of credit hours for the selected classes</t>
-  </si>
-  <si>
     <t>The system should display Class Cards for the selected classes. Class Cards contain the class name, credit hours, instructor, and class length. Each class card should have a unique color</t>
   </si>
   <si>
@@ -98,21 +92,12 @@
     <t>4</t>
   </si>
   <si>
-    <t xml:space="preserve">	</t>
-  </si>
-  <si>
     <t>4.1</t>
   </si>
   <si>
     <t>4.2</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>5.1</t>
-  </si>
-  <si>
     <t>The system should display the currently-selected schedule, with the ability to rotate through all possible permutations if courses offer multiple times.</t>
   </si>
   <si>
@@ -209,52 +194,7 @@
     <t>If there is no valid permutation and unblocking a slot creates one or more valid permutations, one of the now-valid permutations should become selected</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>The user should be able to pin and unpin classes through the UI</t>
-  </si>
-  <si>
-    <t>10.1</t>
-  </si>
-  <si>
-    <t>The user should be able to left-click on a schedule card to pin it to its current time</t>
-  </si>
-  <si>
-    <t>10.2</t>
-  </si>
-  <si>
-    <t>When a schedule card is pinned, it should show a pin icon in the top-right</t>
-  </si>
-  <si>
-    <t>10.3</t>
-  </si>
-  <si>
-    <t>The user should be able to unpin a schedule card by left-clicking it</t>
-  </si>
-  <si>
-    <t>10.4</t>
-  </si>
-  <si>
-    <t>All schedule cards displaying a common class section number should share their pinned status</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>The user should be able to block times through the UI, and should receive feedback from the UI for which times are blocked</t>
-  </si>
-  <si>
-    <t>11.1</t>
-  </si>
-  <si>
-    <t>The user should be able to block and unblock times by right-clicking on a time slot and dragging over any times they want to toggle the status of</t>
-  </si>
-  <si>
-    <t>11.2</t>
-  </si>
-  <si>
-    <t>The UI should darken out the time slots to reflect them being blocked.</t>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -408,12 +348,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -449,6 +383,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -787,7 +727,7 @@
   <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,35 +757,37 @@
     </row>
     <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="H2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="8"/>
     </row>
     <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -853,471 +795,467 @@
       <c r="D3">
         <v>6</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="13"/>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="11"/>
     </row>
     <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="13"/>
+      <c r="C4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="15"/>
+    </row>
+    <row r="6" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="17"/>
+    </row>
+    <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5"/>
-      <c r="H5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="17"/>
-    </row>
-    <row r="6" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="6">
-        <v>3</v>
-      </c>
-      <c r="D6" s="6">
-        <v>7</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="19"/>
-    </row>
-    <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="5">
-        <v>2</v>
-      </c>
-      <c r="D8" s="5">
-        <v>8</v>
+      <c r="A8" s="4">
+        <v>7.1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>7</v>
+        <v>7.2</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>10</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C10" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>7.1</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="4">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4">
-        <v>9</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>7.2</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="4">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4">
-        <v>10</v>
-      </c>
-      <c r="E11" s="4"/>
+      <c r="C11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>7.3</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="C13" s="4">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4">
+        <v>11</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>7.3</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="4">
-        <v>5</v>
-      </c>
-      <c r="D15" s="4">
-        <v>11</v>
-      </c>
-      <c r="E15" s="4"/>
+      <c r="C15" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="C16" s="4">
+        <v>3</v>
+      </c>
+      <c r="D16" s="4">
+        <v>12</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="C17" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="4">
-        <v>3</v>
-      </c>
-      <c r="D18" s="4">
-        <v>12</v>
-      </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="C19" s="5">
+        <v>5</v>
+      </c>
+      <c r="D19" s="5">
+        <v>13</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="C20" s="5">
+        <v>2</v>
+      </c>
+      <c r="D20" s="5">
+        <v>14</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D21" s="5">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="5">
-        <v>2</v>
-      </c>
-      <c r="D22" s="5">
-        <v>14</v>
+      <c r="C22" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="5">
-        <v>3</v>
-      </c>
-      <c r="D23" s="5">
-        <v>15</v>
+      <c r="C23" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
+      <c r="C24" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="4">
-        <v>3</v>
-      </c>
-      <c r="D27" s="4">
-        <v>17</v>
-      </c>
-      <c r="E27" s="4"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="5">
-        <v>3</v>
-      </c>
-      <c r="D32" s="5">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+    </row>
+    <row r="35" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>